<commit_message>
added digestion, density separation, and sampling apparatus columns to data.xlsx; need to add data to the cells
</commit_message>
<xml_diff>
--- a/code/validator/www/data.xlsx
+++ b/code/validator/www/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/One4All/code/validator/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D07302-A460-0041-AFDF-2CE6211160D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99FC580-07AA-3C46-ABB2-273ABA813009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="methodology" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="159">
   <si>
     <t>SamplingDevice</t>
   </si>
@@ -481,6 +481,24 @@
   </si>
   <si>
     <t>SampleComments</t>
+  </si>
+  <si>
+    <t>SampleApparatus</t>
+  </si>
+  <si>
+    <t>DigestionSolutionComposition</t>
+  </si>
+  <si>
+    <t>DigestionConcentration</t>
+  </si>
+  <si>
+    <t>DigestionTemperature</t>
+  </si>
+  <si>
+    <t>DensitySeparationDensity</t>
+  </si>
+  <si>
+    <t>DensitySeparationComposition</t>
   </si>
 </sst>
 </file>
@@ -1178,11 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomLeft" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1208,7 @@
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1263,8 +1281,23 @@
       <c r="X1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1335,7 +1368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1406,7 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1508,9 +1541,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
@@ -1522,7 +1555,7 @@
     <col min="8" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -1566,10 +1599,13 @@
         <v>56</v>
       </c>
       <c r="O1" t="s">
+        <v>153</v>
+      </c>
+      <c r="P1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1613,7 +1649,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
@@ -1657,7 +1693,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>71</v>
       </c>
@@ -1701,7 +1737,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>72</v>
       </c>
@@ -1745,7 +1781,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>73</v>
       </c>
@@ -1789,7 +1825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>74</v>
       </c>
@@ -1833,7 +1869,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>75</v>
       </c>
@@ -1877,7 +1913,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>76</v>
       </c>
@@ -1921,7 +1957,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>77</v>
       </c>
@@ -1965,7 +2001,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
@@ -2011,7 +2047,7 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="textLength" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G2:G11 B2:E11 M2:N11 J2:J11" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="textLength" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G2:G11 B2:E11 M2:O11 J2:J11" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G11" xr:uid="{00000000-0002-0000-0400-000006000000}">
@@ -13678,25 +13714,25 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B2:B242">
-    <cfRule type="containsText" dxfId="25" priority="80" operator="containsText" text=".pdf">
-      <formula>NOT(ISERROR(SEARCH(".pdf", B2)))</formula>
+    <cfRule type="containsText" dxfId="25" priority="76" operator="containsText" text="www">
+      <formula>NOT(ISERROR(SEARCH("www", B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="79" operator="containsText" text="ftp">
-      <formula>NOT(ISERROR(SEARCH("ftp", B2)))</formula>
+    <cfRule type="containsText" dxfId="24" priority="77" operator="containsText" text="https">
+      <formula>NOT(ISERROR(SEARCH("https", B2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="23" priority="78" operator="containsText" text="http">
       <formula>NOT(ISERROR(SEARCH("http", B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="77" operator="containsText" text="https">
-      <formula>NOT(ISERROR(SEARCH("https", B2)))</formula>
+    <cfRule type="containsText" dxfId="22" priority="79" operator="containsText" text="ftp">
+      <formula>NOT(ISERROR(SEARCH("ftp", B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="76" operator="containsText" text="www">
-      <formula>NOT(ISERROR(SEARCH("www", B2)))</formula>
+    <cfRule type="containsText" dxfId="21" priority="80" operator="containsText" text=".pdf">
+      <formula>NOT(ISERROR(SEARCH(".pdf", B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E242">
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text=".jpg">
-      <formula>NOT(ISERROR(SEARCH(".jpg", D2)))</formula>
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="www">
+      <formula>NOT(ISERROR(SEARCH("www", D2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="https">
       <formula>NOT(ISERROR(SEARCH("https", D2)))</formula>
@@ -13710,55 +13746,55 @@
     <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text=".png">
       <formula>NOT(ISERROR(SEARCH(".png", D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="www">
-      <formula>NOT(ISERROR(SEARCH("www", D2)))</formula>
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text=".jpg">
+      <formula>NOT(ISERROR(SEARCH(".jpg", D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G242">
-    <cfRule type="containsText" dxfId="14" priority="60" operator="containsText" text=".zip">
+    <cfRule type="containsText" dxfId="14" priority="55" operator="containsText" text="www">
+      <formula>NOT(ISERROR(SEARCH("www", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="56" operator="containsText" text="https">
+      <formula>NOT(ISERROR(SEARCH("https", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="57" operator="containsText" text="http">
+      <formula>NOT(ISERROR(SEARCH("http", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="58" operator="containsText" text="ftp">
+      <formula>NOT(ISERROR(SEARCH("ftp", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="59" operator="containsText" text=".">
+      <formula>NOT(ISERROR(SEARCH(".", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="60" operator="containsText" text=".zip">
       <formula>NOT(ISERROR(SEARCH(".zip", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="61" operator="containsText" text=".yaml">
+    <cfRule type="containsText" dxfId="8" priority="61" operator="containsText" text=".yaml">
       <formula>NOT(ISERROR(SEARCH(".yaml", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="59" operator="containsText" text=".">
-      <formula>NOT(ISERROR(SEARCH(".", G2)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="62" operator="containsText" text=".json">
+      <formula>NOT(ISERROR(SEARCH(".json", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="63" operator="containsText" text=".qs">
+    <cfRule type="containsText" dxfId="6" priority="63" operator="containsText" text=".qs">
       <formula>NOT(ISERROR(SEARCH(".qs", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="64" operator="containsText" text=".rds">
+    <cfRule type="containsText" dxfId="5" priority="64" operator="containsText" text=".rds">
       <formula>NOT(ISERROR(SEARCH(".rds", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="65" operator="containsText" text=".jdx">
+    <cfRule type="containsText" dxfId="4" priority="65" operator="containsText" text=".jdx">
       <formula>NOT(ISERROR(SEARCH(".jdx", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="66" operator="containsText" text=".spc">
+    <cfRule type="containsText" dxfId="3" priority="66" operator="containsText" text=".spc">
       <formula>NOT(ISERROR(SEARCH(".spc", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="67" operator="containsText" text=".spa">
+    <cfRule type="containsText" dxfId="2" priority="67" operator="containsText" text=".spa">
       <formula>NOT(ISERROR(SEARCH(".spa", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="68" operator="containsText" text=".asp">
+    <cfRule type="containsText" dxfId="1" priority="68" operator="containsText" text=".asp">
       <formula>NOT(ISERROR(SEARCH(".asp", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="69" operator="containsText" text=".csv">
+    <cfRule type="containsText" dxfId="0" priority="69" operator="containsText" text=".csv">
       <formula>NOT(ISERROR(SEARCH(".csv", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="58" operator="containsText" text="ftp">
-      <formula>NOT(ISERROR(SEARCH("ftp", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="57" operator="containsText" text="http">
-      <formula>NOT(ISERROR(SEARCH("http", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="56" operator="containsText" text="https">
-      <formula>NOT(ISERROR(SEARCH("https", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="55" operator="containsText" text="www">
-      <formula>NOT(ISERROR(SEARCH("www", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="62" operator="containsText" text=".json">
-      <formula>NOT(ISERROR(SEARCH(".json", G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>

<commit_message>
added 'Sieving' to data.xlsx
</commit_message>
<xml_diff>
--- a/code/validator/www/data.xlsx
+++ b/code/validator/www/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/One4All/code/validator/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99FC580-07AA-3C46-ABB2-273ABA813009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F0A05D-0B4B-FC4C-B23E-783EE0A81C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="methodology" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="160">
   <si>
     <t>SamplingDevice</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>DensitySeparationComposition</t>
+  </si>
+  <si>
+    <t>Sieving</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AD1" sqref="AD1"/>
     </sheetView>
@@ -1543,9 +1546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1648,6 +1651,9 @@
       <c r="N2" t="s">
         <v>52</v>
       </c>
+      <c r="O2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1692,6 +1698,9 @@
       <c r="N3" t="s">
         <v>52</v>
       </c>
+      <c r="O3" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1736,6 +1745,9 @@
       <c r="N4" t="s">
         <v>52</v>
       </c>
+      <c r="O4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1780,6 +1792,9 @@
       <c r="N5" t="s">
         <v>52</v>
       </c>
+      <c r="O5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1824,6 +1839,9 @@
       <c r="N6" t="s">
         <v>52</v>
       </c>
+      <c r="O6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -1868,6 +1886,9 @@
       <c r="N7" t="s">
         <v>52</v>
       </c>
+      <c r="O7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -1912,6 +1933,9 @@
       <c r="N8" t="s">
         <v>52</v>
       </c>
+      <c r="O8" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1956,6 +1980,9 @@
       <c r="N9" t="s">
         <v>52</v>
       </c>
+      <c r="O9" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -2000,6 +2027,9 @@
       <c r="N10" t="s">
         <v>52</v>
       </c>
+      <c r="O10" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -2044,10 +2074,13 @@
       <c r="N11" t="s">
         <v>52</v>
       </c>
+      <c r="O11" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="textLength" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G2:G11 B2:E11 M2:O11 J2:J11" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="textLength" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="G2:G11 B2:E11 J2:J11 M2:O11" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G11" xr:uid="{00000000-0002-0000-0400-000006000000}">
@@ -13714,25 +13747,25 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B2:B242">
-    <cfRule type="containsText" dxfId="25" priority="76" operator="containsText" text="www">
-      <formula>NOT(ISERROR(SEARCH("www", B2)))</formula>
+    <cfRule type="containsText" dxfId="25" priority="80" operator="containsText" text=".pdf">
+      <formula>NOT(ISERROR(SEARCH(".pdf", B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="77" operator="containsText" text="https">
-      <formula>NOT(ISERROR(SEARCH("https", B2)))</formula>
+    <cfRule type="containsText" dxfId="24" priority="79" operator="containsText" text="ftp">
+      <formula>NOT(ISERROR(SEARCH("ftp", B2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="23" priority="78" operator="containsText" text="http">
       <formula>NOT(ISERROR(SEARCH("http", B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="79" operator="containsText" text="ftp">
-      <formula>NOT(ISERROR(SEARCH("ftp", B2)))</formula>
+    <cfRule type="containsText" dxfId="22" priority="77" operator="containsText" text="https">
+      <formula>NOT(ISERROR(SEARCH("https", B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="80" operator="containsText" text=".pdf">
-      <formula>NOT(ISERROR(SEARCH(".pdf", B2)))</formula>
+    <cfRule type="containsText" dxfId="21" priority="76" operator="containsText" text="www">
+      <formula>NOT(ISERROR(SEARCH("www", B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E242">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="www">
-      <formula>NOT(ISERROR(SEARCH("www", D2)))</formula>
+    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text=".jpg">
+      <formula>NOT(ISERROR(SEARCH(".jpg", D2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="https">
       <formula>NOT(ISERROR(SEARCH("https", D2)))</formula>
@@ -13746,55 +13779,55 @@
     <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text=".png">
       <formula>NOT(ISERROR(SEARCH(".png", D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text=".jpg">
-      <formula>NOT(ISERROR(SEARCH(".jpg", D2)))</formula>
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="www">
+      <formula>NOT(ISERROR(SEARCH("www", D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G242">
-    <cfRule type="containsText" dxfId="14" priority="55" operator="containsText" text="www">
+    <cfRule type="containsText" dxfId="14" priority="60" operator="containsText" text=".zip">
+      <formula>NOT(ISERROR(SEARCH(".zip", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="61" operator="containsText" text=".yaml">
+      <formula>NOT(ISERROR(SEARCH(".yaml", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="59" operator="containsText" text=".">
+      <formula>NOT(ISERROR(SEARCH(".", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="63" operator="containsText" text=".qs">
+      <formula>NOT(ISERROR(SEARCH(".qs", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="64" operator="containsText" text=".rds">
+      <formula>NOT(ISERROR(SEARCH(".rds", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="65" operator="containsText" text=".jdx">
+      <formula>NOT(ISERROR(SEARCH(".jdx", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="66" operator="containsText" text=".spc">
+      <formula>NOT(ISERROR(SEARCH(".spc", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="67" operator="containsText" text=".spa">
+      <formula>NOT(ISERROR(SEARCH(".spa", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="68" operator="containsText" text=".asp">
+      <formula>NOT(ISERROR(SEARCH(".asp", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="69" operator="containsText" text=".csv">
+      <formula>NOT(ISERROR(SEARCH(".csv", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="58" operator="containsText" text="ftp">
+      <formula>NOT(ISERROR(SEARCH("ftp", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="57" operator="containsText" text="http">
+      <formula>NOT(ISERROR(SEARCH("http", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="56" operator="containsText" text="https">
+      <formula>NOT(ISERROR(SEARCH("https", G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="55" operator="containsText" text="www">
       <formula>NOT(ISERROR(SEARCH("www", G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="56" operator="containsText" text="https">
-      <formula>NOT(ISERROR(SEARCH("https", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="57" operator="containsText" text="http">
-      <formula>NOT(ISERROR(SEARCH("http", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="58" operator="containsText" text="ftp">
-      <formula>NOT(ISERROR(SEARCH("ftp", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="59" operator="containsText" text=".">
-      <formula>NOT(ISERROR(SEARCH(".", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="60" operator="containsText" text=".zip">
-      <formula>NOT(ISERROR(SEARCH(".zip", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="61" operator="containsText" text=".yaml">
-      <formula>NOT(ISERROR(SEARCH(".yaml", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="62" operator="containsText" text=".json">
+    <cfRule type="containsText" dxfId="0" priority="62" operator="containsText" text=".json">
       <formula>NOT(ISERROR(SEARCH(".json", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="63" operator="containsText" text=".qs">
-      <formula>NOT(ISERROR(SEARCH(".qs", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="64" operator="containsText" text=".rds">
-      <formula>NOT(ISERROR(SEARCH(".rds", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="65" operator="containsText" text=".jdx">
-      <formula>NOT(ISERROR(SEARCH(".jdx", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="66" operator="containsText" text=".spc">
-      <formula>NOT(ISERROR(SEARCH(".spc", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="67" operator="containsText" text=".spa">
-      <formula>NOT(ISERROR(SEARCH(".spa", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="68" operator="containsText" text=".asp">
-      <formula>NOT(ISERROR(SEARCH(".asp", G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="69" operator="containsText" text=".csv">
-      <formula>NOT(ISERROR(SEARCH(".csv", G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>